<commit_message>
Añadida planificacion del Sprint 2
</commit_message>
<xml_diff>
--- a/planning.xlsx
+++ b/planning.xlsx
@@ -3,14 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlo\OneDrive\Escritorio\DP 2021\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{165A045C-31E2-4FBA-948C-E63887912491}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{611B20B4-5CA5-4359-96F2-06467CFF02C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{E13FE9D1-DD16-4DD8-A01D-AAE97F59CC2A}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="20760" windowHeight="11820" activeTab="2" xr2:uid="{E13FE9D1-DD16-4DD8-A01D-AAE97F59CC2A}"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="1" r:id="rId1"/>
@@ -21,7 +16,8 @@
     <sheet name="Sprint 5" sheetId="6" r:id="rId6"/>
     <sheet name="Sprint 6" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:H17"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="27">
   <si>
     <t>Fecha</t>
   </si>
@@ -105,13 +101,28 @@
   </si>
   <si>
     <t>Planificado</t>
+  </si>
+  <si>
+    <t>Sprint 2 - ITEM 2 A CGR</t>
+  </si>
+  <si>
+    <t>Sprint 2 - ITEM 2 B CGR</t>
+  </si>
+  <si>
+    <t>Sprint 2 - ITEM 3</t>
+  </si>
+  <si>
+    <t>Sprint 2 - ITEM 1</t>
+  </si>
+  <si>
+    <t>Sprint2 - ITEM 2 A JVG</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -144,6 +155,14 @@
     <font>
       <b/>
       <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -306,7 +325,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -335,26 +354,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -773,99 +798,99 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA7D2506-CDFC-4856-A39A-20D8BFB61BF5}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" style="10" customWidth="1"/>
-    <col min="2" max="2" width="47.140625" style="10" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="10"/>
-    <col min="4" max="5" width="11.42578125" style="10" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="10"/>
+    <col min="1" max="1" width="13.5703125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="47.140625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="9"/>
+    <col min="4" max="5" width="11.42578125" style="9" customWidth="1"/>
+    <col min="6" max="16384" width="11.42578125" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="11"/>
+      <c r="B1" s="14"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="16">
+      <c r="B2" s="11">
         <v>44115</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="12"/>
+      <c r="B3" s="13"/>
     </row>
     <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
-      <c r="B4" s="9"/>
+      <c r="A4" s="12"/>
+      <c r="B4" s="12"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="15"/>
+      <c r="B5" s="16"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="13"/>
+      <c r="B6" s="15"/>
     </row>
     <row r="7" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="9"/>
+      <c r="B7" s="12"/>
     </row>
     <row r="8" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="9"/>
+      <c r="B8" s="12"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="13"/>
+      <c r="B9" s="15"/>
     </row>
     <row r="10" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="9"/>
+      <c r="B10" s="12"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="9"/>
+      <c r="B11" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -874,81 +899,111 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94513516-0377-4E36-A178-A8E01AF17E14}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" style="10" customWidth="1"/>
-    <col min="2" max="2" width="47.140625" style="10" customWidth="1"/>
-    <col min="3" max="16384" width="11.42578125" style="10"/>
+    <col min="1" max="1" width="13.5703125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="47.140625" style="9" customWidth="1"/>
+    <col min="3" max="16384" width="11.42578125" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="11"/>
+      <c r="B1" s="14"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="16">
+      <c r="B2" s="11">
         <v>44123</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="12"/>
+      <c r="B3" s="13"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
-      <c r="B4" s="9"/>
+      <c r="A4" s="12"/>
+      <c r="B4" s="12"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="15"/>
+      <c r="B5" s="16"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="13"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
+      <c r="B6" s="15"/>
+    </row>
+    <row r="7" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="12"/>
+    </row>
+    <row r="8" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="12"/>
+    </row>
+    <row r="9" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="12"/>
+    </row>
+    <row r="10" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="13"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
+      <c r="B10" s="15"/>
+    </row>
+    <row r="11" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="12"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="12"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="17"/>
+      <c r="B13" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
+  <mergeCells count="11">
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -962,60 +1017,60 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" style="10" customWidth="1"/>
-    <col min="2" max="2" width="47.140625" style="10" customWidth="1"/>
-    <col min="3" max="16384" width="11.42578125" style="10"/>
+    <col min="1" max="1" width="13.5703125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="47.140625" style="9" customWidth="1"/>
+    <col min="3" max="16384" width="11.42578125" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="11"/>
+      <c r="B1" s="14"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="16">
+      <c r="B2" s="11">
         <v>44129</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="12"/>
+      <c r="B3" s="13"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
-      <c r="B4" s="9"/>
+      <c r="A4" s="12"/>
+      <c r="B4" s="12"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="15"/>
+      <c r="B5" s="16"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="13"/>
+      <c r="B6" s="15"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="12"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="13"/>
+      <c r="B8" s="15"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -1042,60 +1097,60 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" style="10" customWidth="1"/>
-    <col min="2" max="2" width="47.140625" style="10" customWidth="1"/>
-    <col min="3" max="16384" width="11.42578125" style="10"/>
+    <col min="1" max="1" width="13.5703125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="47.140625" style="9" customWidth="1"/>
+    <col min="3" max="16384" width="11.42578125" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="11"/>
+      <c r="B1" s="14"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="16">
+      <c r="B2" s="11">
         <v>44139</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="12"/>
+      <c r="B3" s="13"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
-      <c r="B4" s="9"/>
+      <c r="A4" s="12"/>
+      <c r="B4" s="12"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="15"/>
+      <c r="B5" s="16"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="13"/>
+      <c r="B6" s="15"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="12"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="13"/>
+      <c r="B8" s="15"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -1122,60 +1177,60 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" style="10" customWidth="1"/>
-    <col min="2" max="2" width="47.140625" style="10" customWidth="1"/>
-    <col min="3" max="16384" width="11.42578125" style="10"/>
+    <col min="1" max="1" width="13.5703125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="47.140625" style="9" customWidth="1"/>
+    <col min="3" max="16384" width="11.42578125" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="11"/>
+      <c r="B1" s="14"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="16">
+      <c r="B2" s="11">
         <v>44150</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="12"/>
+      <c r="B3" s="13"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
-      <c r="B4" s="9"/>
+      <c r="A4" s="12"/>
+      <c r="B4" s="12"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="15"/>
+      <c r="B5" s="16"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="13"/>
+      <c r="B6" s="15"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="12"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="13"/>
+      <c r="B8" s="15"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -1202,60 +1257,60 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" style="10" customWidth="1"/>
-    <col min="2" max="2" width="47.140625" style="10" customWidth="1"/>
-    <col min="3" max="16384" width="11.42578125" style="10"/>
+    <col min="1" max="1" width="13.5703125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="47.140625" style="9" customWidth="1"/>
+    <col min="3" max="16384" width="11.42578125" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="11"/>
+      <c r="B1" s="14"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="16">
+      <c r="B2" s="11">
         <v>44157</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="12"/>
+      <c r="B3" s="13"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
-      <c r="B4" s="9"/>
+      <c r="A4" s="12"/>
+      <c r="B4" s="12"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="15"/>
+      <c r="B5" s="16"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="13"/>
+      <c r="B6" s="15"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="12"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="13"/>
+      <c r="B8" s="15"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
Añadida planificación y subida de versión para el nuevo Sprint 3
</commit_message>
<xml_diff>
--- a/planning.xlsx
+++ b/planning.xlsx
@@ -3,9 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{611B20B4-5CA5-4359-96F2-06467CFF02C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlo\OneDrive\Escritorio\DP Diciembre\Workspace-2.19\Acme-FleaMarket\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA808AC2-2EEB-4282-9768-9251F7267396}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="20760" windowHeight="11820" activeTab="2" xr2:uid="{E13FE9D1-DD16-4DD8-A01D-AAE97F59CC2A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="3" xr2:uid="{E13FE9D1-DD16-4DD8-A01D-AAE97F59CC2A}"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="1" r:id="rId1"/>
@@ -17,25 +22,16 @@
     <sheet name="Sprint 6" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:H17"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="32">
   <si>
     <t>Fecha</t>
   </si>
@@ -116,6 +112,21 @@
   </si>
   <si>
     <t>Sprint2 - ITEM 2 A JVG</t>
+  </si>
+  <si>
+    <t>Sprint 3 - ITEM 1</t>
+  </si>
+  <si>
+    <t>Sprint 3 - ITEM 2_A JVG</t>
+  </si>
+  <si>
+    <t>Sprint 3 - ITEM 3</t>
+  </si>
+  <si>
+    <t>Sprint 3 - ITEM 2_A CGR</t>
+  </si>
+  <si>
+    <t>Sprint 3 - ITEM 2_B CGR</t>
   </si>
 </sst>
 </file>
@@ -169,7 +180,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -215,6 +226,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -325,7 +342,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -363,6 +380,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -375,10 +398,13 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -698,7 +724,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -743,7 +769,7 @@
     </row>
     <row r="4" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="6">
-        <v>44129</v>
+        <v>44134</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>5</v>
@@ -754,7 +780,7 @@
     </row>
     <row r="5" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A5" s="6">
-        <v>44139</v>
+        <v>44141</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>6</v>
@@ -798,7 +824,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA7D2506-CDFC-4856-A39A-20D8BFB61BF5}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
@@ -814,10 +840,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="14"/>
+      <c r="B1" s="16"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
@@ -828,69 +854,69 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="13"/>
+      <c r="B3" s="15"/>
     </row>
     <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12"/>
+      <c r="A4" s="19"/>
+      <c r="B4" s="19"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="16"/>
+      <c r="B5" s="18"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="15"/>
+      <c r="B6" s="17"/>
     </row>
     <row r="7" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="12"/>
+      <c r="B7" s="19"/>
     </row>
     <row r="8" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="12"/>
+      <c r="B8" s="19"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="15"/>
+      <c r="B9" s="17"/>
     </row>
     <row r="10" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="12"/>
+      <c r="B10" s="19"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="12"/>
+      <c r="B11" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A4:B4"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A4:B4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -901,7 +927,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94513516-0377-4E36-A178-A8E01AF17E14}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -913,10 +939,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="14"/>
+      <c r="B1" s="16"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
@@ -927,66 +953,66 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="13"/>
+      <c r="B3" s="15"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12"/>
+      <c r="A4" s="19"/>
+      <c r="B4" s="19"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="16"/>
+      <c r="B5" s="18"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="15"/>
-    </row>
-    <row r="7" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+      <c r="B6" s="17"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="12"/>
-    </row>
-    <row r="8" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
+      <c r="B7" s="19"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="12"/>
-    </row>
-    <row r="9" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+      <c r="B8" s="19"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="12"/>
-    </row>
-    <row r="10" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
+      <c r="B9" s="19"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="15"/>
-    </row>
-    <row r="11" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
+      <c r="B10" s="17"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="12"/>
+      <c r="B11" s="19"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="12"/>
+      <c r="B12" s="19"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="17"/>
-      <c r="B13" s="18"/>
+      <c r="A13" s="13"/>
+      <c r="B13" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -1009,10 +1035,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06E4A99C-8EA1-4651-B11E-825C3254766F}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1023,67 +1049,100 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="14"/>
+      <c r="B1" s="16"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="11">
-        <v>44129</v>
+        <v>44134</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="13"/>
+      <c r="B3" s="15"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12"/>
+      <c r="A4" s="19"/>
+      <c r="B4" s="19"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="16"/>
+      <c r="B5" s="18"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="15"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="12"/>
-      <c r="B7" s="12"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
+      <c r="B6" s="17"/>
+    </row>
+    <row r="7" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="20"/>
+    </row>
+    <row r="8" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="20"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="19"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="15"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
+      <c r="B10" s="17"/>
+    </row>
+    <row r="11" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="20"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="19"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
+  <mergeCells count="12">
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A12:B12"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A9:B9"/>
     <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A11:B11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1092,7 +1151,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1103,54 +1162,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="14"/>
+      <c r="B1" s="16"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="11">
-        <v>44139</v>
+        <v>44141</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="13"/>
+      <c r="B3" s="15"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12"/>
+      <c r="A4" s="19"/>
+      <c r="B4" s="19"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="16"/>
+      <c r="B5" s="18"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="15"/>
+      <c r="B6" s="17"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="12"/>
-      <c r="B7" s="12"/>
+      <c r="A7" s="19"/>
+      <c r="B7" s="19"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="15"/>
+      <c r="B8" s="17"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
+      <c r="A9" s="19"/>
+      <c r="B9" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -1183,10 +1242,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="14"/>
+      <c r="B1" s="16"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
@@ -1197,40 +1256,40 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="13"/>
+      <c r="B3" s="15"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12"/>
+      <c r="A4" s="19"/>
+      <c r="B4" s="19"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="16"/>
+      <c r="B5" s="18"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="15"/>
+      <c r="B6" s="17"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="12"/>
-      <c r="B7" s="12"/>
+      <c r="A7" s="19"/>
+      <c r="B7" s="19"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="15"/>
+      <c r="B8" s="17"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
+      <c r="A9" s="19"/>
+      <c r="B9" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -1263,10 +1322,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="14"/>
+      <c r="B1" s="16"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
@@ -1277,40 +1336,40 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="13"/>
+      <c r="B3" s="15"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12"/>
+      <c r="A4" s="19"/>
+      <c r="B4" s="19"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="16"/>
+      <c r="B5" s="18"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="15"/>
+      <c r="B6" s="17"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="12"/>
-      <c r="B7" s="12"/>
+      <c r="A7" s="19"/>
+      <c r="B7" s="19"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="15"/>
+      <c r="B8" s="17"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
+      <c r="A9" s="19"/>
+      <c r="B9" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>